<commit_message>
[Feat:KSW] Add MapPrefabs & Add MonsterWeapon
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterWeaponInfo.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterWeaponInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{378D4AB0-32A6-4D06-8799-817CC052DF20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF6591D-F215-4EBF-8E84-9003F04DAD86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12180" xr2:uid="{54B67A6B-0125-404E-858E-6A0D8AE0942A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>key</t>
   </si>
@@ -135,6 +135,10 @@
   </si>
   <si>
     <t>SoliderWeapon</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BodyWeapon</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -526,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362566D3-E1DC-47B9-A3CF-83840ACFA7D9}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -705,6 +709,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Fix:KSW] Fix WoodType Weapon Attack
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterWeaponInfo.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/MonsterWeaponInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\TheLegendoftheArcher_8team\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF6591D-F215-4EBF-8E84-9003F04DAD86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBAC205-69E8-4CB9-86AD-7799BE52DD53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12180" xr2:uid="{54B67A6B-0125-404E-858E-6A0D8AE0942A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>key</t>
   </si>
@@ -139,6 +139,10 @@
   </si>
   <si>
     <t>BodyWeapon</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -533,7 +537,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -737,6 +741,9 @@
       <c r="I6">
         <v>0.1</v>
       </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>